<commit_message>
completed schematic + layout, generated production files
</commit_message>
<xml_diff>
--- a/Project Outputs for minesweeper-mainboard/BOM/Bill of Materials-minesweeper-mainboard.xlsx
+++ b/Project Outputs for minesweeper-mainboard/BOM/Bill of Materials-minesweeper-mainboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/649dfdc13902ec6b/Desktop/IGEN-430-Minesweeper/Project Outputs for minesweeper-mainboard/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="8_{58562CAF-7E85-491D-952E-78E2AE5205A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5B4B41A-8D52-4BBB-AB8C-EE5435AE34CF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E2A6614-3CFD-4913-B2BB-680A3928A0C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A6751522-E539-4D90-839E-CCA76CE553DF}"/>
+    <workbookView xWindow="5865" yWindow="285" windowWidth="21600" windowHeight="11385" xr2:uid="{8969A47E-046D-4301-A719-C1762F438CEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-minesweeper-m" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="164">
   <si>
     <t>Comment</t>
   </si>
@@ -128,12 +128,18 @@
     <t>0.10uF</t>
   </si>
   <si>
-    <t>C13, C14, C15, C24, C25</t>
+    <t>C13, C14</t>
+  </si>
+  <si>
+    <t>0603</t>
   </si>
   <si>
     <t>CAP 0.1uF 50V</t>
   </si>
   <si>
+    <t>C15, C24, C25</t>
+  </si>
+  <si>
     <t>4.7uF</t>
   </si>
   <si>
@@ -179,21 +185,12 @@
     <t>LED;Red;11mcd;0.061In.Dia.;SMD;100mA;2V Vf;635nm;140deg;SMD;White Diffused;5V Vr | Lumex SML-LXT0805IW-TR</t>
   </si>
   <si>
-    <t>D2, D6, D7, D8, D9</t>
+    <t>D2, D3, D6, D7, D8, D9</t>
   </si>
   <si>
     <t>LEDC2012X120N</t>
   </si>
   <si>
-    <t>SML-LXT0805GW-TR</t>
-  </si>
-  <si>
-    <t>Green LED, 565 nm 0805Diffused, Rectangle Lens SMD package | Lumex SML-LXT0805GW-TR</t>
-  </si>
-  <si>
-    <t>D3</t>
-  </si>
-  <si>
     <t>SM5817PL-TP</t>
   </si>
   <si>
@@ -404,22 +401,37 @@
     <t>1k</t>
   </si>
   <si>
-    <t>R10, R13, R15</t>
-  </si>
-  <si>
-    <t>RES 1.1k 1/8W, RES 1k 1/8W</t>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>RES 1.1k 1/8W</t>
   </si>
   <si>
     <t>10k</t>
   </si>
   <si>
-    <t>RES SMD 10K OHM 1% 1/8W 0603, RES SMD 10K OHM 5% 1/8W 0603, Default Resistor Symbol</t>
-  </si>
-  <si>
-    <t>R11, R12, R17, R23, R26, R27, R28, R29, R30, R31, R32, R33, R34, R35, R36, R37, R38</t>
-  </si>
-  <si>
-    <t>RES 10k 1/8W - 1%, RES 10k 1/8W - 5%</t>
+    <t>RES SMD 10K OHM 1% 1/8W 0603, Default Resistor Symbol</t>
+  </si>
+  <si>
+    <t>R11, R12, R26, R27, R28, R29, R30, R31, R32, R33, R34, R35, R36, R37, R38, R39, R40, R41, R42</t>
+  </si>
+  <si>
+    <t>RES 10k 1/8W - 1%</t>
+  </si>
+  <si>
+    <t>R13, R15</t>
+  </si>
+  <si>
+    <t>RES 1k 1/8W</t>
+  </si>
+  <si>
+    <t>RES SMD 10K OHM 5% 1/8W 0603</t>
+  </si>
+  <si>
+    <t>R17, R23</t>
+  </si>
+  <si>
+    <t>RES 10k 1/8W - 5%</t>
   </si>
   <si>
     <t>YC248-JR-070RL</t>
@@ -519,49 +531,13 @@
   </si>
   <si>
     <t>SOP65P640X120-24N</t>
-  </si>
-  <si>
-    <t>Provided by JLCPCB</t>
-  </si>
-  <si>
-    <t>Not by JLCPCB</t>
-  </si>
-  <si>
-    <t>Digikey</t>
-  </si>
-  <si>
-    <t>Debug pads</t>
-  </si>
-  <si>
-    <t>Battery connector already purchased</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/en/products/detail/c-k/JS202011JAQN/6137629</t>
-  </si>
-  <si>
-    <t>Stepper driver module already acquired</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/en/products/detail/w%C3%BCrth-elektronik/150080VS75000/4489924</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/en/products/detail/diodes-incorporated/SMAZ12-13-F/725035?s=N4IgTCBcDaIMoFkCCAtAjGAtGgzJgYiALoC%2BQA</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/en/products/detail/pulse-electronics/PA4342-682NLT/5641801</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/en/products/detail/w%C3%BCrth-elektronik/61300411121/4846827</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/en/products/detail/sullins-connector-solutions/PPTC202LFBN-RC/807240?s=N4IgTCBcDaIDoBcAEBlAbARgAwBYC0AcgCIgC6AvkA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -569,16 +545,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -588,12 +556,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD3D3D3"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -622,11 +584,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -638,37 +599,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -997,26 +932,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{405D4D6B-FCAE-4DB2-B4CC-980F0F9B9BC7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75C26796-9014-4ECF-BDAA-B0D34777FADF}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="6" width="19.7109375" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" customWidth="1"/>
-    <col min="8" max="8" width="28.42578125" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1035,17 +964,8 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -1064,16 +984,8 @@
       <c r="F2" s="4">
         <v>24</v>
       </c>
-      <c r="G2" s="5" t="str">
-        <f>IF(AND(ISBLANK(H2), ISBLANK(I2)), "Provided", "Not Provided")</f>
-        <v>Not Provided</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="I2" s="5"/>
-    </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -1092,14 +1004,8 @@
       <c r="F3" s="4">
         <v>4</v>
       </c>
-      <c r="G3" s="9" t="str">
-        <f>IF(AND(ISBLANK(H3), ISBLANK(I3)), "Provided", "Not Provided")</f>
-        <v>Provided</v>
-      </c>
-      <c r="H3" s="8"/>
-      <c r="I3" s="5"/>
-    </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
@@ -1118,14 +1024,8 @@
       <c r="F4" s="4">
         <v>2</v>
       </c>
-      <c r="G4" s="9" t="str">
-        <f t="shared" ref="G3:G41" si="0">IF(AND(ISBLANK(H4), ISBLANK(I4)), "Provided", "Not Provided")</f>
-        <v>Provided</v>
-      </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="5"/>
-    </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
@@ -1144,14 +1044,8 @@
       <c r="F5" s="4">
         <v>4</v>
       </c>
-      <c r="G5" s="9" t="str">
-        <f>IF(AND(ISBLANK(H5), ISBLANK(I5)), "Provided", "Not Provided")</f>
-        <v>Provided</v>
-      </c>
-      <c r="H5" s="8"/>
-      <c r="I5" s="5"/>
-    </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
@@ -1170,14 +1064,8 @@
       <c r="F6" s="4">
         <v>1</v>
       </c>
-      <c r="G6" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>Provided</v>
-      </c>
-      <c r="H6" s="8"/>
-      <c r="I6" s="5"/>
-    </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>24</v>
       </c>
@@ -1196,14 +1084,8 @@
       <c r="F7" s="4">
         <v>2</v>
       </c>
-      <c r="G7" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>Provided</v>
-      </c>
-      <c r="H7" s="8"/>
-      <c r="I7" s="5"/>
-    </row>
-    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>28</v>
       </c>
@@ -1214,671 +1096,507 @@
         <v>29</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F8" s="4">
-        <v>5</v>
-      </c>
-      <c r="G8" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>Provided</v>
-      </c>
-      <c r="H8" s="8"/>
-      <c r="I8" s="5"/>
-    </row>
-    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="4">
+      <c r="C10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="4">
         <v>1</v>
       </c>
-      <c r="G9" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>Provided</v>
-      </c>
-      <c r="H9" s="8"/>
-      <c r="I9" s="5"/>
-    </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="3" t="s">
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="4">
+      <c r="C11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="4">
         <v>7</v>
       </c>
-      <c r="G10" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>Provided</v>
-      </c>
-      <c r="H10" s="8"/>
-      <c r="I10" s="5"/>
-    </row>
-    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="3" t="s">
+    </row>
+    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="B12" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="4">
+      <c r="D12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="4">
         <v>1</v>
       </c>
-      <c r="G11" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Not Provided</v>
-      </c>
-      <c r="H11" s="8"/>
-      <c r="I11" s="7" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="3" t="s">
+    </row>
+    <row r="13" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="B13" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F12" s="4">
-        <v>5</v>
-      </c>
-      <c r="G12" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>Provided</v>
-      </c>
-      <c r="H12" s="8"/>
-      <c r="I12" s="5"/>
-    </row>
-    <row r="13" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="E13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F13" s="4">
-        <v>1</v>
-      </c>
-      <c r="G13" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Not Provided</v>
-      </c>
-      <c r="H13" s="8"/>
-      <c r="I13" s="7" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="B14" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="F14" s="4">
         <v>2</v>
       </c>
-      <c r="G14" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>Provided</v>
-      </c>
-      <c r="H14" s="8"/>
-      <c r="I14" s="5"/>
-    </row>
-    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="F15" s="4">
         <v>1</v>
       </c>
-      <c r="G15" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>Provided</v>
-      </c>
-      <c r="H15" s="8"/>
-      <c r="I15" s="5"/>
-    </row>
-    <row r="16" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>64</v>
-      </c>
       <c r="E16" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F16" s="4">
         <v>2</v>
       </c>
-      <c r="G16" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Not Provided</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="I16" s="5"/>
-    </row>
-    <row r="17" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="E17" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F17" s="4">
         <v>8</v>
       </c>
-      <c r="G17" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>Provided</v>
-      </c>
-      <c r="H17" s="8"/>
-      <c r="I17" s="5"/>
-    </row>
-    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>72</v>
-      </c>
       <c r="E18" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F18" s="4">
         <v>1</v>
       </c>
-      <c r="G18" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>Not Provided</v>
-      </c>
-      <c r="H18" s="8"/>
-      <c r="I18" s="7" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="E19" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F19" s="4">
         <v>3</v>
       </c>
-      <c r="G19" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>Provided</v>
-      </c>
-      <c r="H19" s="8"/>
-      <c r="I19" s="5"/>
-    </row>
-    <row r="20" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>80</v>
-      </c>
       <c r="E20" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F20" s="4">
         <v>1</v>
       </c>
-      <c r="G20" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Not Provided</v>
-      </c>
-      <c r="H20" s="8"/>
-      <c r="I20" s="7" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="E21" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>85</v>
       </c>
       <c r="F21" s="4">
         <v>1</v>
       </c>
-      <c r="G21" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Not Provided</v>
-      </c>
-      <c r="H21" s="8"/>
-      <c r="I21" s="7" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="E22" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>90</v>
       </c>
       <c r="F22" s="4">
         <v>1</v>
       </c>
-      <c r="G22" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Not Provided</v>
-      </c>
-      <c r="H22" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="I22" s="5"/>
-    </row>
-    <row r="23" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>95</v>
       </c>
       <c r="F23" s="4">
         <v>2</v>
       </c>
-      <c r="G23" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>Provided</v>
-      </c>
-      <c r="H23" s="8"/>
-      <c r="I23" s="5"/>
-    </row>
-    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>99</v>
-      </c>
       <c r="E24" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F24" s="4">
         <v>4</v>
       </c>
-      <c r="G24" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>Provided</v>
-      </c>
-      <c r="H24" s="8"/>
-      <c r="I24" s="5"/>
-    </row>
-    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>102</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F25" s="4">
         <v>2</v>
       </c>
-      <c r="G25" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>Provided</v>
-      </c>
-      <c r="H25" s="8"/>
-      <c r="I25" s="5"/>
-    </row>
-    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F26" s="4">
         <v>4</v>
       </c>
-      <c r="G26" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>Provided</v>
-      </c>
-      <c r="H26" s="8"/>
-      <c r="I26" s="5"/>
-    </row>
-    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>108</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F27" s="4">
         <v>1</v>
       </c>
-      <c r="G27" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>Provided</v>
-      </c>
-      <c r="H27" s="8"/>
-      <c r="I27" s="5"/>
-    </row>
-    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>111</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F28" s="4">
         <v>1</v>
       </c>
-      <c r="G28" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>Provided</v>
-      </c>
-      <c r="H28" s="8"/>
-      <c r="I28" s="5"/>
-    </row>
-    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>115</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F29" s="4">
         <v>1</v>
       </c>
-      <c r="G29" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>Provided</v>
-      </c>
-      <c r="H29" s="8"/>
-      <c r="I29" s="5"/>
-    </row>
-    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>117</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>118</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F30" s="4">
         <v>5</v>
       </c>
-      <c r="G30" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>Provided</v>
-      </c>
-      <c r="H30" s="8"/>
-      <c r="I30" s="5"/>
-    </row>
-    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>120</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>121</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E31" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="F31" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="F31" s="4">
-        <v>3</v>
-      </c>
-      <c r="G31" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>Provided</v>
-      </c>
-      <c r="H31" s="8"/>
-      <c r="I31" s="5"/>
-    </row>
-    <row r="32" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+      <c r="B32" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="C32" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>125</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E32" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F32" s="4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="F32" s="4">
-        <v>17</v>
-      </c>
-      <c r="G32" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>Provided</v>
-      </c>
-      <c r="H32" s="8"/>
-      <c r="I32" s="5"/>
-    </row>
-    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>128</v>
-      </c>
       <c r="D33" s="3" t="s">
-        <v>129</v>
+        <v>30</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>127</v>
@@ -1886,79 +1604,59 @@
       <c r="F33" s="4">
         <v>2</v>
       </c>
-      <c r="G33" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>Provided</v>
-      </c>
-      <c r="H33" s="8"/>
-      <c r="I33" s="5"/>
-    </row>
-    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E34" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>132</v>
       </c>
       <c r="F34" s="4">
         <v>2</v>
       </c>
-      <c r="G34" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>Provided</v>
-      </c>
-      <c r="H34" s="8"/>
-      <c r="I34" s="5"/>
-    </row>
-    <row r="35" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>134</v>
+        <v>96</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>133</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F35" s="4">
-        <v>1</v>
-      </c>
-      <c r="G35" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Not Provided</v>
-      </c>
-      <c r="H35" s="8"/>
-      <c r="I35" s="7" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>137</v>
+        <v>100</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>139</v>
+        <v>13</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>136</v>
@@ -1966,161 +1664,150 @@
       <c r="F36" s="4">
         <v>2</v>
       </c>
-      <c r="G36" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>Provided</v>
-      </c>
-      <c r="H36" s="8"/>
-      <c r="I36" s="5"/>
-    </row>
-    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>97</v>
+        <v>138</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="F37" s="4">
         <v>1</v>
       </c>
-      <c r="G37" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>Provided</v>
-      </c>
-      <c r="H37" s="8"/>
-      <c r="I37" s="5"/>
-    </row>
-    <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F38" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B39" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="D39" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="E39" s="3" t="s">
         <v>147</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="F38" s="4">
-        <v>1</v>
-      </c>
-      <c r="G38" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>Provided</v>
-      </c>
-      <c r="H38" s="8"/>
-      <c r="I38" s="5"/>
-    </row>
-    <row r="39" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>148</v>
       </c>
       <c r="F39" s="4">
         <v>1</v>
       </c>
-      <c r="G39" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Not Provided</v>
-      </c>
-      <c r="H39" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="I39" s="5"/>
-    </row>
-    <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F40" s="4">
         <v>1</v>
       </c>
-      <c r="G40" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>Provided</v>
-      </c>
-      <c r="H40" s="8"/>
-      <c r="I40" s="5"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="F41" s="4">
         <v>1</v>
       </c>
-      <c r="G41" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>Provided</v>
-      </c>
-      <c r="H41" s="8"/>
-      <c r="I41" s="5"/>
+    </row>
+    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F42" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="F43" s="4">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G2:G41">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>"Enter the formula: =AND(ISBLANK($H$2:$H$41), ISBLANK($I$2:$I$41))"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <hyperlinks>
-    <hyperlink ref="I35" r:id="rId1" xr:uid="{9914DD83-A518-4502-A0C0-ABC0304BD1AA}"/>
-    <hyperlink ref="I13" r:id="rId2" xr:uid="{0BDD9957-7A10-4E7F-ADD9-D86BA8F4CE55}"/>
-    <hyperlink ref="I11" r:id="rId3" xr:uid="{8D65D1D4-BCA3-4B8D-92C5-2DC446C927D5}"/>
-    <hyperlink ref="I21" r:id="rId4" xr:uid="{BBE3F463-BC1A-4A74-90DA-84283745FA9C}"/>
-    <hyperlink ref="I20" r:id="rId5" xr:uid="{B4250C20-9138-4C3B-A94E-FCAF07A3E358}"/>
-    <hyperlink ref="I18" r:id="rId6" xr:uid="{431EFD45-5CE9-4E3B-8ABE-B9180670AFE1}"/>
-  </hyperlinks>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup scale="33" orientation="landscape" blackAndWhite="1" r:id="rId7"/>
+  <pageSetup scale="33" orientation="landscape" blackAndWhite="1" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>